<commit_message>
First runable Version includes printing
</commit_message>
<xml_diff>
--- a/Code/data/Dummy Scenarios.xlsx
+++ b/Code/data/Dummy Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wmd852\Documents\Doktorantenkurse\Ketter\Code_Gruppenabgabe\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9287FAF8-B324-4E92-93C7-9EE27D862652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5A6A62-0207-4D17-9AA1-C403036282FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-105" windowWidth="30930" windowHeight="16920" xr2:uid="{154585FB-EFC7-48CF-82C2-38CED2C866E8}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37470" windowHeight="18210" xr2:uid="{154585FB-EFC7-48CF-82C2-38CED2C866E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="4" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>lambda_D</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>O_D</t>
-  </si>
-  <si>
     <t>P_t_S</t>
   </si>
   <si>
@@ -91,6 +88,24 @@
   </si>
   <si>
     <t>Zeros</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>O_Rank</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>Spalte2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spalte_43 </t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -159,14 +174,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -185,8 +222,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="6" xr16:uid="{714B5327-EE1A-478E-97A9-843B0FC8C79B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="17" unboundColumnsRight="2">
-    <queryTableFields count="13">
+  <queryTableRefresh nextId="24" unboundColumnsRight="7">
+    <queryTableFields count="18">
       <queryTableField id="9" name="Index" tableColumnId="9"/>
       <queryTableField id="1" name="lambda_D" tableColumnId="1"/>
       <queryTableField id="2" name="P_tau" tableColumnId="2"/>
@@ -200,18 +237,23 @@
       <queryTableField id="8" name="r_minus" tableColumnId="8"/>
       <queryTableField id="11" dataBound="0" tableColumnId="10"/>
       <queryTableField id="16" dataBound="0" tableColumnId="13"/>
+      <queryTableField id="17" dataBound="0" tableColumnId="14"/>
+      <queryTableField id="20" dataBound="0" tableColumnId="15"/>
+      <queryTableField id="21" dataBound="0" tableColumnId="16"/>
+      <queryTableField id="22" dataBound="0" tableColumnId="17"/>
+      <queryTableField id="23" dataBound="0" tableColumnId="18"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9B286734-B18E-4800-A67D-A8F95AA75A8A}" name="Results" displayName="Results" ref="A1:M65" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M65" xr:uid="{85A3FCE3-7AC5-4FED-AEA0-EDB441BFF35E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9B286734-B18E-4800-A67D-A8F95AA75A8A}" name="Results" displayName="Results" ref="A1:R66" tableType="queryTable" totalsRowCount="1">
+  <autoFilter ref="A1:R65" xr:uid="{85A3FCE3-7AC5-4FED-AEA0-EDB441BFF35E}"/>
   <sortState ref="A2:L65">
     <sortCondition ref="B1:B65"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="18">
     <tableColumn id="9" xr3:uid="{CC50FD64-BE59-4162-96BC-FACA10369F94}" uniqueName="9" name="Index" queryTableFieldId="9"/>
     <tableColumn id="1" xr3:uid="{6E5C56EF-CFDC-4883-B925-CAED5B2745C5}" uniqueName="1" name="lambda_D" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{B3C182D3-1DD1-438E-ACC3-B6346F947E99}" uniqueName="2" name="P_tau" queryTableFieldId="2"/>
@@ -223,10 +265,24 @@
     <tableColumn id="11" xr3:uid="{B5068C9F-528B-4F51-A584-8B43D5D380D7}" uniqueName="11" name="P_t_S" queryTableFieldId="12"/>
     <tableColumn id="12" xr3:uid="{F057473B-4975-4C90-8FC5-0E8A9BDF6334}" uniqueName="12" name="P_t_W" queryTableFieldId="13"/>
     <tableColumn id="8" xr3:uid="{736949D7-562F-4981-ACB9-FE8CD6DA55DC}" uniqueName="8" name="r_minus" queryTableFieldId="8"/>
-    <tableColumn id="10" xr3:uid="{2E8A8233-582E-4B2B-8666-CE721387D246}" uniqueName="10" name="O_D" queryTableFieldId="11" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{2E8A8233-582E-4B2B-8666-CE721387D246}" uniqueName="10" name="O_Rank" queryTableFieldId="11" dataDxfId="7" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Results[[#This Row],[lambda_D]]=20,1,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{A37B0388-5B36-4C80-96A7-ED770D359DE6}" uniqueName="13" name="Zeros" queryTableFieldId="16"/>
+    <tableColumn id="14" xr3:uid="{9126A2D3-E1DB-40AB-B216-B11851C7F0AC}" uniqueName="14" name="Pi" queryTableFieldId="17" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{72D7096A-DCEE-47BB-8E28-30292974292D}" uniqueName="15" name="Spalte1" queryTableFieldId="20" dataDxfId="5">
+      <calculatedColumnFormula>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{E95C2532-17D9-440F-A4D7-9E0A97CF017A}" uniqueName="16" name="Spalte2" queryTableFieldId="21" dataDxfId="4">
+      <calculatedColumnFormula>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{84274DF1-BB5F-4AEB-A57D-4E9D9CBA7A73}" uniqueName="17" name="Spalte_43 " queryTableFieldId="22" dataDxfId="3">
+      <calculatedColumnFormula>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{2041740B-C09E-4067-B596-B4008F287099}" uniqueName="18" name="Result" totalsRowFunction="custom" queryTableFieldId="23" dataDxfId="2">
+      <calculatedColumnFormula>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Results[Result])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -585,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1464F757-9524-4B61-BC60-1FEC87231C34}">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:E48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +662,7 @@
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -632,22 +688,37 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25</v>
       </c>
@@ -688,8 +759,27 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O2">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P2" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R2" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>26</v>
       </c>
@@ -730,8 +820,27 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O3">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P3" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R3" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>27</v>
       </c>
@@ -772,8 +881,27 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O4">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P4" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R4" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
@@ -814,8 +942,27 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O5">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P5" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R5" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29</v>
       </c>
@@ -856,8 +1003,27 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0.26</v>
+      </c>
+      <c r="O6">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P6" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R6" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -898,8 +1064,27 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0.26</v>
+      </c>
+      <c r="O7">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P7" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R7" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>31</v>
       </c>
@@ -940,8 +1125,27 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0.26</v>
+      </c>
+      <c r="O8">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P8" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R8" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
@@ -982,8 +1186,27 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0.26</v>
+      </c>
+      <c r="O9">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P9" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q9" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R9" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>33</v>
       </c>
@@ -1024,8 +1247,27 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O10">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P10" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R10" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -1066,8 +1308,27 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O11">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P11" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q11" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R11" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
@@ -1108,8 +1369,27 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O12">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P12" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q12" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R12" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>36</v>
       </c>
@@ -1150,8 +1430,27 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O13">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P13" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R13" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>37</v>
       </c>
@@ -1192,8 +1491,27 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>0.26</v>
+      </c>
+      <c r="O14">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P14" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q14" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R14" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>38</v>
       </c>
@@ -1234,8 +1552,27 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>0.26</v>
+      </c>
+      <c r="O15">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P15" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R15" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>39</v>
       </c>
@@ -1276,8 +1613,27 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0.26</v>
+      </c>
+      <c r="O16">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P16" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R16" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1318,8 +1674,27 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0.26</v>
+      </c>
+      <c r="O17">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P17" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q17" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R17" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>49</v>
       </c>
@@ -1360,8 +1735,27 @@
       <c r="M18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O18">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P18" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R18" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>50</v>
       </c>
@@ -1402,8 +1796,27 @@
       <c r="M19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O19">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P19" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q19" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R19" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>51</v>
       </c>
@@ -1444,8 +1857,27 @@
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O20">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P20" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q20" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R20" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>52</v>
       </c>
@@ -1486,8 +1918,27 @@
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O21">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P21" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q21" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R21" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>53</v>
       </c>
@@ -1528,8 +1979,27 @@
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>0.26</v>
+      </c>
+      <c r="O22">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P22" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q22" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R22" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>54</v>
       </c>
@@ -1570,8 +2040,27 @@
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>0.26</v>
+      </c>
+      <c r="O23">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P23" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q23" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R23" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>55</v>
       </c>
@@ -1612,8 +2101,27 @@
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>0.26</v>
+      </c>
+      <c r="O24">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P24" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q24" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R24" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>56</v>
       </c>
@@ -1654,8 +2162,27 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0.26</v>
+      </c>
+      <c r="O25">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P25" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q25" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R25" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>57</v>
       </c>
@@ -1696,8 +2223,27 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O26">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P26" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q26" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R26" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>58</v>
       </c>
@@ -1738,8 +2284,27 @@
       <c r="M27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O27">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P27" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q27" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R27" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>59</v>
       </c>
@@ -1780,8 +2345,27 @@
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O28">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P28" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q28" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R28" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>60</v>
       </c>
@@ -1822,8 +2406,27 @@
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="O29">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P29" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q29" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R29" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>61</v>
       </c>
@@ -1864,8 +2467,27 @@
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>0.26</v>
+      </c>
+      <c r="O30">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P30" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q30" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R30" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>62</v>
       </c>
@@ -1906,8 +2528,27 @@
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>0.26</v>
+      </c>
+      <c r="O31">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P31" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R31" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>63</v>
       </c>
@@ -1948,8 +2589,27 @@
       <c r="M32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>0.26</v>
+      </c>
+      <c r="O32">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P32" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q32" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R32" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>64</v>
       </c>
@@ -1990,8 +2650,27 @@
       <c r="M33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>0.26</v>
+      </c>
+      <c r="O33">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P33" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q33" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R33" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2032,8 +2711,27 @@
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>0.21</v>
+      </c>
+      <c r="O34">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P34" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q34" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R34" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2074,8 +2772,27 @@
       <c r="M35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>0.21</v>
+      </c>
+      <c r="O35">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P35" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q35" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R35" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2116,8 +2833,27 @@
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>0.21</v>
+      </c>
+      <c r="O36">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P36" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q36" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R36" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2158,8 +2894,27 @@
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>0.21</v>
+      </c>
+      <c r="O37">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P37" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q37" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R37" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2200,8 +2955,27 @@
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>0.39</v>
+      </c>
+      <c r="O38">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P38" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q38" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R38" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -2242,8 +3016,27 @@
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>0.39</v>
+      </c>
+      <c r="O39">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P39" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q39" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R39" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2284,8 +3077,27 @@
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>0.39</v>
+      </c>
+      <c r="O40">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P40" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q40" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R40" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2326,8 +3138,27 @@
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>0.39</v>
+      </c>
+      <c r="O41">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P41" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q41" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R41" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2368,8 +3199,27 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>0.21</v>
+      </c>
+      <c r="O42">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P42" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q42" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R42" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
@@ -2410,8 +3260,27 @@
       <c r="M43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>0.21</v>
+      </c>
+      <c r="O43">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P43" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q43" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R43" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11</v>
       </c>
@@ -2452,8 +3321,27 @@
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>0.21</v>
+      </c>
+      <c r="O44">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P44" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q44" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R44" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12</v>
       </c>
@@ -2494,8 +3382,27 @@
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>0.21</v>
+      </c>
+      <c r="O45">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P45" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q45" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R45" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>13</v>
       </c>
@@ -2536,8 +3443,27 @@
       <c r="M46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>0.39</v>
+      </c>
+      <c r="O46">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P46" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q46" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R46" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -2578,8 +3504,27 @@
       <c r="M47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>0.39</v>
+      </c>
+      <c r="O47">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P47" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q47" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R47" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15</v>
       </c>
@@ -2620,8 +3565,27 @@
       <c r="M48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>0.39</v>
+      </c>
+      <c r="O48">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P48" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q48" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R48" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>16</v>
       </c>
@@ -2662,8 +3626,27 @@
       <c r="M49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>0.39</v>
+      </c>
+      <c r="O49">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P49" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R49" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>17</v>
       </c>
@@ -2704,8 +3687,27 @@
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>0.21</v>
+      </c>
+      <c r="O50">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P50" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R50" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>18</v>
       </c>
@@ -2746,8 +3748,27 @@
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>0.21</v>
+      </c>
+      <c r="O51">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P51" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q51" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R51" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>19</v>
       </c>
@@ -2788,8 +3809,27 @@
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>0.21</v>
+      </c>
+      <c r="O52">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P52" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q52" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R52" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20</v>
       </c>
@@ -2830,8 +3870,27 @@
       <c r="M53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>0.21</v>
+      </c>
+      <c r="O53">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P53" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q53" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R53" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>21</v>
       </c>
@@ -2872,8 +3931,27 @@
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>0.39</v>
+      </c>
+      <c r="O54">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P54" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q54" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R54" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>22</v>
       </c>
@@ -2914,8 +3992,27 @@
       <c r="M55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>0.39</v>
+      </c>
+      <c r="O55">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P55" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q55" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R55" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>23</v>
       </c>
@@ -2956,8 +4053,27 @@
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>0.39</v>
+      </c>
+      <c r="O56">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P56" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q56" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R56" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>24</v>
       </c>
@@ -2998,8 +4114,27 @@
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>0.39</v>
+      </c>
+      <c r="O57">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P57" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q57" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R57" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>41</v>
       </c>
@@ -3040,8 +4175,27 @@
       <c r="M58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>0.21</v>
+      </c>
+      <c r="O58">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P58" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q58" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R58" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>42</v>
       </c>
@@ -3082,8 +4236,27 @@
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>0.21</v>
+      </c>
+      <c r="O59">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P59" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q59" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R59" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>43</v>
       </c>
@@ -3124,8 +4297,27 @@
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>0.21</v>
+      </c>
+      <c r="O60">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P60" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q60" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R60" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>44</v>
       </c>
@@ -3166,8 +4358,27 @@
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>0.21</v>
+      </c>
+      <c r="O61">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P61" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.35</v>
+      </c>
+      <c r="Q61" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R61" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>45</v>
       </c>
@@ -3208,8 +4419,27 @@
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>0.39</v>
+      </c>
+      <c r="O62">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P62" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q62" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R62" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>46</v>
       </c>
@@ -3250,8 +4480,27 @@
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>0.39</v>
+      </c>
+      <c r="O63">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P63" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q63" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R63" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>47</v>
       </c>
@@ -3292,8 +4541,27 @@
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>0.39</v>
+      </c>
+      <c r="O64">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P64" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q64" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R64" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>48</v>
       </c>
@@ -3333,6 +4601,33 @@
       </c>
       <c r="M65">
         <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0.39</v>
+      </c>
+      <c r="O65">
+        <f>IF(Results[[#This Row],[lambda_D]],0.6,0.4)</f>
+        <v>0.6</v>
+      </c>
+      <c r="P65" s="2">
+        <f>IF(Results[[#This Row],[lambda_D]]-Results[[#This Row],[lambda_A]]=10,0.35,0.6)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q65" s="2">
+        <f>IF(Results[[#This Row],[r_minus]]=1.5,0.7,0.3)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R65" s="2">
+        <f>Results[[#This Row],[Spalte1]]*Results[[#This Row],[Spalte2]]*Results[[#This Row],[Spalte_43 ]]</f>
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="R66">
+        <f>SUM(Results[Result])</f>
+        <v>9.1199999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>